<commit_message>
Corrected one wrong time
</commit_message>
<xml_diff>
--- a/raw-data/Timetable_Master_Management.xlsx
+++ b/raw-data/Timetable_Master_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Lo Priore\Documents\MASTER 2.1\Programming\project--G2\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F7F574-37C3-4654-B9F0-E01C234B9488}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A92302-2BAD-45B2-B96F-03C327B72614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{7D46FA66-D2EE-D643-A8C9-830764CAC309}"/>
   </bookViews>
@@ -987,7 +987,7 @@
     <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>14</v>
       </c>
       <c r="J27" s="3">
-        <v>0.5</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="K27" s="3">
         <v>0.58333333333333337</v>
@@ -2111,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>2</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>2</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>2</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>2</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>2</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>2</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>2</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>2</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>2</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>3</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>3</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>3</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>3</v>
       </c>
@@ -5065,9 +5065,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M99" xr:uid="{FF6BCF00-F687-40BD-9D06-559784E76804}">
-    <filterColumn colId="2">
+    <filterColumn colId="7">
       <filters>
-        <filter val="International Strategy"/>
+        <filter val="12.50"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>